<commit_message>
update spreadsheet for FSAD
</commit_message>
<xml_diff>
--- a/resources/CS-Module-Marks-Tracker-blank.xlsx
+++ b/resources/CS-Module-Marks-Tracker-blank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\matth\Documents\school\UNI\Birmingham\Comp. Sci\CS Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\matth\Documents\school\UNI\Birmingham\Comp. Sci\CS Resources\FirstYearCSResources\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C64B75-E091-4629-899D-E3F5D24E8E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5E66D0-FDFC-4B27-B5EE-6051F84AB81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="13" xr2:uid="{B7EF9BA6-F1C8-4970-808A-2941F4194624}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{B7EF9BA6-F1C8-4970-808A-2941F4194624}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="7" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="120">
   <si>
     <t>Module</t>
   </si>
@@ -407,6 +407,9 @@
   </si>
   <si>
     <t>Maths &amp; Logic in Comp. Sci.</t>
+  </si>
+  <si>
+    <t>Assignment 1</t>
   </si>
 </sst>
 </file>
@@ -534,7 +537,115 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="75">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -572,34 +683,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -628,34 +711,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -715,27 +770,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -2736,15 +2770,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>20411</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>42182</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>265386</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>124811</xdr:rowOff>
+      <xdr:colOff>285797</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>166993</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2760,8 +2794,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="190500"/>
-          <a:ext cx="1484586" cy="505811"/>
+          <a:off x="1098097" y="1261382"/>
+          <a:ext cx="1669643" cy="505811"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3274,16 +3308,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{20D3C205-D24B-481F-A0A5-97A6101B312A}" name="DSA" displayName="DSA" ref="A2:G7" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{20D3C205-D24B-481F-A0A5-97A6101B312A}" name="DSA" displayName="DSA" ref="A2:G7" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
   <autoFilter ref="A2:G7" xr:uid="{20D3C205-D24B-481F-A0A5-97A6101B312A}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2270E0A8-E28C-4AF9-BFC1-A412E0725E4C}" name="Assessment" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{7052E14A-65AF-43E2-8483-D779564FD6C0}" name="Type" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{63A96BCC-5661-4CA8-9927-9E1FA068D3C4}" name="Date" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{1F33FCAA-DEEE-45E2-89E6-03E71911E17F}" name="Weight" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{F1F6B912-427B-4B79-AD72-0E5794AA2EB0}" name="Marks" dataDxfId="59"/>
-    <tableColumn id="6" xr3:uid="{C6CD4014-F914-41A7-9044-7D2D5C20AB20}" name="Out Of" dataDxfId="58"/>
-    <tableColumn id="7" xr3:uid="{21C62A9F-30A4-4FEA-9205-6025E71D32F4}" name="Percent" dataDxfId="57">
+    <tableColumn id="1" xr3:uid="{2270E0A8-E28C-4AF9-BFC1-A412E0725E4C}" name="Assessment" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{7052E14A-65AF-43E2-8483-D779564FD6C0}" name="Type" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{63A96BCC-5661-4CA8-9927-9E1FA068D3C4}" name="Date" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{1F33FCAA-DEEE-45E2-89E6-03E71911E17F}" name="Weight" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{F1F6B912-427B-4B79-AD72-0E5794AA2EB0}" name="Marks" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{C6CD4014-F914-41A7-9044-7D2D5C20AB20}" name="Out Of" dataDxfId="67"/>
+    <tableColumn id="7" xr3:uid="{21C62A9F-30A4-4FEA-9205-6025E71D32F4}" name="Percent" dataDxfId="66">
       <calculatedColumnFormula>IFERROR(DSA[[#This Row],[Marks]]/DSA[[#This Row],[Out Of]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3292,16 +3326,34 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B4AFA088-5628-4B0C-A947-DF271B3597BC}" name="MLFCS" displayName="MLFCS" ref="A2:G15" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F35ED7B2-2694-475F-9750-DB6006F821CB}" name="OOP_9" displayName="OOP_9" ref="A2:G5" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A2:G5" xr:uid="{F35ED7B2-2694-475F-9750-DB6006F821CB}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{E80B8A59-3B9F-4512-8A91-0C6601A07EE2}" name="Assessment" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{E5D6FFF2-E218-4868-ADD3-69587A76F673}" name="Type" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{59C1D46E-21B1-49C7-8032-C8F8375176BE}" name="Date" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{74073497-F8B4-4CA4-AE6C-18AF43D79BB4}" name="Weight" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{E1196646-88EC-4C14-B54C-30FABBD9067B}" name="Marks" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{F7783659-DAB3-47F3-B843-4B680178AE5A}" name="Out Of" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{63276932-3C7D-439A-979B-4B0ECD257653}" name="Percent" dataDxfId="11">
+      <calculatedColumnFormula>IFERROR(OOP_9[[#This Row],[Marks]]/OOP_9[[#This Row],[Out Of]],0)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B4AFA088-5628-4B0C-A947-DF271B3597BC}" name="MLFCS" displayName="MLFCS" ref="A2:G15" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
   <autoFilter ref="A2:G15" xr:uid="{B4AFA088-5628-4B0C-A947-DF271B3597BC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{15DC20F1-D841-4813-BF61-022F87C55DD2}" name="Assessment" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{98565EC1-AB66-491E-907F-60B1C3C06AED}" name="Type" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{E226E69F-80DF-46D2-B2DB-919F4093C819}" name="Date" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{14002C37-7FC0-4B1E-9971-2BD856C2B2DB}" name="Weight" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{4896E73E-0ED6-41FF-AEF7-13DD8D5F34A7}" name="Marks" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{1D2BE4DF-6511-493E-AE36-FF8A538CC8FF}" name="Out Of" dataDxfId="49"/>
-    <tableColumn id="7" xr3:uid="{C9A7BCBC-9AE4-4642-AEA7-952B70FD4E74}" name="Percent" dataDxfId="48">
+    <tableColumn id="1" xr3:uid="{15DC20F1-D841-4813-BF61-022F87C55DD2}" name="Assessment" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{98565EC1-AB66-491E-907F-60B1C3C06AED}" name="Type" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{E226E69F-80DF-46D2-B2DB-919F4093C819}" name="Date" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{14002C37-7FC0-4B1E-9971-2BD856C2B2DB}" name="Weight" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{4896E73E-0ED6-41FF-AEF7-13DD8D5F34A7}" name="Marks" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{1D2BE4DF-6511-493E-AE36-FF8A538CC8FF}" name="Out Of" dataDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{C9A7BCBC-9AE4-4642-AEA7-952B70FD4E74}" name="Percent" dataDxfId="57">
       <calculatedColumnFormula>IFERROR(MLFCS[[#This Row],[Marks]]/MLFCS[[#This Row],[Out Of]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3309,17 +3361,17 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2622BBBF-6102-430C-9085-5B9BC95AF7B6}" name="OOP" displayName="OOP" ref="A2:G10" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2622BBBF-6102-430C-9085-5B9BC95AF7B6}" name="OOP" displayName="OOP" ref="A2:G10" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
   <autoFilter ref="A2:G10" xr:uid="{2622BBBF-6102-430C-9085-5B9BC95AF7B6}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8AF69D61-70B0-4B62-8A94-84FFD4FF1E30}" name="Assessment" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{6115B625-2524-4C13-BFC6-76AD80B08F00}" name="Type" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{8E7F7644-5258-47D7-BE01-F1673A9FC9F3}" name="Date" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{A9B92261-E9DB-46C0-9F8E-65E2E3C608F6}" name="Weight" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{CB9AA16B-15AA-4947-B2F6-F7C81AF67420}" name="Marks" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{9B24B904-A5F0-44D1-ACED-E4E0338FA6DF}" name="Out Of" dataDxfId="40"/>
-    <tableColumn id="7" xr3:uid="{1A8558B6-1346-45CB-8F71-8D91CA9265F5}" name="Percent" dataDxfId="39">
+    <tableColumn id="1" xr3:uid="{8AF69D61-70B0-4B62-8A94-84FFD4FF1E30}" name="Assessment" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{6115B625-2524-4C13-BFC6-76AD80B08F00}" name="Type" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{8E7F7644-5258-47D7-BE01-F1673A9FC9F3}" name="Date" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{A9B92261-E9DB-46C0-9F8E-65E2E3C608F6}" name="Weight" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{CB9AA16B-15AA-4947-B2F6-F7C81AF67420}" name="Marks" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{9B24B904-A5F0-44D1-ACED-E4E0338FA6DF}" name="Out Of" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{1A8558B6-1346-45CB-8F71-8D91CA9265F5}" name="Percent" dataDxfId="48">
       <calculatedColumnFormula>IFERROR(OOP[[#This Row],[Marks]]/OOP[[#This Row],[Out Of]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3327,63 +3379,63 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C7F83F0-696F-4DA9-816E-95829FA77043}" name="Table1" displayName="Table1" ref="A2:E14" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C7F83F0-696F-4DA9-816E-95829FA77043}" name="Table1" displayName="Table1" ref="A2:E14" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A2:E14" xr:uid="{8C7F83F0-696F-4DA9-816E-95829FA77043}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E14">
     <sortCondition ref="C2:C14"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8D63AB25-C4F5-4F25-B996-68DBB88FA60D}" name="Module" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{1C29305E-3227-4597-BBEC-44A2B0E4CC4F}" name="Credits" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{B27A0533-DD77-42EF-8198-23242DE0BD7D}" name="Year" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{4D8DE3E4-490E-4E79-85EE-043DF7F56F53}" name="Semester" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{7AE710B2-1596-40DF-AA87-0DC058FAF3E4}" name="Total" dataDxfId="29"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}" name="Table5" displayName="Table5" ref="A1:E27" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
-  <autoFilter ref="A1:E27" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E27">
-    <sortCondition ref="D1:D27"/>
-  </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{45B78292-D524-4642-96FC-D0DF620F1A72}" name="Assessment" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{1CA06CD8-476D-4D7E-B485-B99253CDAB02}" name="Module" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{8951D55B-B6A3-4963-B426-3FFB2CC407BA}" name="Weight" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{8DF606BA-0DF3-4A1F-93E7-16047639F3B4}" name="Release" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{7E03F087-A839-4404-AF22-222490C90F19}" name="Due" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{8D63AB25-C4F5-4F25-B996-68DBB88FA60D}" name="Module" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{1C29305E-3227-4597-BBEC-44A2B0E4CC4F}" name="Credits" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{B27A0533-DD77-42EF-8198-23242DE0BD7D}" name="Year" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{4D8DE3E4-490E-4E79-85EE-043DF7F56F53}" name="Semester" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{7AE710B2-1596-40DF-AA87-0DC058FAF3E4}" name="Total" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}" name="FYModules" displayName="FYModules" ref="A2:D16" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A2:D16" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7F7F705C-BBFB-48B0-B110-926E8E1CF419}" name="Name" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{99F42913-A4AF-439C-AFDE-38735B9668A7}" name="Semester 1" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{140A5CE5-3F0E-4A39-9385-36A06BB6BA02}" name="Semester 2" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{B24B6960-A926-4304-9414-949D710BDB68}" name="Select?" dataDxfId="12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}" name="Table5" displayName="Table5" ref="A1:E27" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+  <autoFilter ref="A1:E27" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E27">
+    <sortCondition ref="D1:D27"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{45B78292-D524-4642-96FC-D0DF620F1A72}" name="Assessment" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{1CA06CD8-476D-4D7E-B485-B99253CDAB02}" name="Module" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{8951D55B-B6A3-4963-B426-3FFB2CC407BA}" name="Weight" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{8DF606BA-0DF3-4A1F-93E7-16047639F3B4}" name="Release" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{7E03F087-A839-4404-AF22-222490C90F19}" name="Due" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{788C9EAD-B8A7-4E97-A5AD-984A0BD58BD0}" name="CyberSecModules" displayName="CyberSecModules" ref="A2:F11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}" name="FYModules" displayName="FYModules" ref="A2:D16" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="A2:D16" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{7F7F705C-BBFB-48B0-B110-926E8E1CF419}" name="Name" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{99F42913-A4AF-439C-AFDE-38735B9668A7}" name="Semester 1" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{140A5CE5-3F0E-4A39-9385-36A06BB6BA02}" name="Semester 2" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{B24B6960-A926-4304-9414-949D710BDB68}" name="Select?" dataDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{788C9EAD-B8A7-4E97-A5AD-984A0BD58BD0}" name="CyberSecModules" displayName="CyberSecModules" ref="A2:F11" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A2:F11" xr:uid="{788C9EAD-B8A7-4E97-A5AD-984A0BD58BD0}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D2F9F639-DE00-4891-82FC-F2AFD9BED136}" name="Name" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{4A6B316E-C867-46CE-9E04-295046356E23}" name="Type" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{C3FB9A35-9CAA-490E-B5DD-3FB2B7EAFF24}" name="Autumn" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{7E3D05E3-EEED-4E51-9F2B-7A430A5FFFF9}" name="Spring" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{CC9BCECD-842A-4322-8A50-9292CE0AE138}" name="Summer" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{E6BCA339-BC30-44BF-9D15-3F15733224FF}" name="Select?" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D2F9F639-DE00-4891-82FC-F2AFD9BED136}" name="Name" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{4A6B316E-C867-46CE-9E04-295046356E23}" name="Type" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{C3FB9A35-9CAA-490E-B5DD-3FB2B7EAFF24}" name="Autumn" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{7E3D05E3-EEED-4E51-9F2B-7A430A5FFFF9}" name="Spring" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{CC9BCECD-842A-4322-8A50-9292CE0AE138}" name="Summer" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{E6BCA339-BC30-44BF-9D15-3F15733224FF}" name="Select?" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3811,8 +3863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FB547B-EB02-4962-87B0-376B1EBB9A6D}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4044,13 +4096,13 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E14">
-    <cfRule type="containsBlanks" dxfId="38" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="10" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThanOrEqual">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="lessThan">
       <formula>0.4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4828,18 +4880,18 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="equal">
       <formula>120</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="20" priority="4" operator="notContains" text="120">
+    <cfRule type="notContainsText" dxfId="6" priority="4" operator="notContains" text="120">
       <formula>ISERROR(SEARCH("120",G5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G4">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="notEqual">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>60</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5156,18 +5208,18 @@
     <mergeCell ref="H2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>180</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>180</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>60</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5199,7 +5251,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E6"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5437,16 +5489,208 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC581F71-13EA-4CC9-8894-8953E0805102}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D9:D10"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="4">
+        <v>44634</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6">
+        <v>100</v>
+      </c>
+      <c r="G3" s="5">
+        <f>IFERROR(OOP_9[[#This Row],[Marks]]/OOP_9[[#This Row],[Out Of]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="7">
+        <f>SUMIF(OOP_9[Type],"AS",OOP_9[Weight])</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="7">
+        <f>(SUMIF(OOP_9[Type],"AS",OOP_9[Percent]))/COUNTIF(OOP_9[Type],"AS")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="4">
+        <v>44684</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6">
+        <v>100</v>
+      </c>
+      <c r="G4" s="5">
+        <f>IFERROR(OOP_9[[#This Row],[Marks]]/OOP_9[[#This Row],[Out Of]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="7">
+        <f>SUM(J3:J3)</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="7">
+        <f>(J3*K3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="4">
+        <v>44697</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6">
+        <v>100</v>
+      </c>
+      <c r="G5" s="5">
+        <f>IFERROR(OOP_9[[#This Row],[Marks]]/OOP_9[[#This Row],[Out Of]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -5862,8 +6106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694825E1-042E-4FA4-8770-4069ED8A6469}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E10"/>
+    <sheetView topLeftCell="B1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection sqref="A1:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update spreadsheet for FSAD and AI
</commit_message>
<xml_diff>
--- a/resources/CS-Module-Marks-Tracker-blank.xlsx
+++ b/resources/CS-Module-Marks-Tracker-blank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\matth\Documents\school\UNI\Birmingham\Comp. Sci\CS Resources\FirstYearCSResources\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5E66D0-FDFC-4B27-B5EE-6051F84AB81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60B0E0C-8368-4161-9A75-CDCC73DFF335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{B7EF9BA6-F1C8-4970-808A-2941F4194624}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7EF9BA6-F1C8-4970-808A-2941F4194624}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="7" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="122">
   <si>
     <t>Module</t>
   </si>
@@ -410,6 +410,12 @@
   </si>
   <si>
     <t>Assignment 1</t>
+  </si>
+  <si>
+    <t>Quiz 5</t>
+  </si>
+  <si>
+    <t>Quizzes</t>
   </si>
 </sst>
 </file>
@@ -537,7 +543,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="75">
+  <dxfs count="84">
     <dxf>
       <fill>
         <patternFill>
@@ -614,37 +620,6 @@
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -770,6 +745,68 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -2567,16 +2604,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>191894</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>165875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>236811</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>124811</xdr:rowOff>
+      <xdr:colOff>657305</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>100186</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2592,8 +2629,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="581025" y="190500"/>
-          <a:ext cx="1484586" cy="505811"/>
+          <a:off x="1269845" y="1954716"/>
+          <a:ext cx="2017289" cy="505811"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3308,6 +3345,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9EA4CCE4-E406-4481-AA90-9A07CAD5BE7E}" name="OOP_10" displayName="OOP_10" ref="A2:G8" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+  <autoFilter ref="A2:G8" xr:uid="{9EA4CCE4-E406-4481-AA90-9A07CAD5BE7E}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{69A62117-FC87-4ECC-AB98-EF35B05A468E}" name="Assessment" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{60753137-725D-4636-8C02-EC3D7FD23525}" name="Type" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{05971888-5882-46B9-8195-7C40FE55BDBF}" name="Date" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{79E72D4D-8ED7-4B0C-8D4A-E1F6B54F9E04}" name="Weight" dataDxfId="78"/>
+    <tableColumn id="5" xr3:uid="{25BA5AEC-6E95-498F-9617-9DADAFA4F49D}" name="Marks" dataDxfId="77"/>
+    <tableColumn id="6" xr3:uid="{8BC298BB-3525-4A67-928C-CDEF4817E4CE}" name="Out Of" dataDxfId="76"/>
+    <tableColumn id="7" xr3:uid="{AD958F54-11F6-4131-85C7-2EB5FF82A984}" name="Percent" dataDxfId="75">
+      <calculatedColumnFormula>IFERROR(OOP_10[[#This Row],[Marks]]/OOP_10[[#This Row],[Out Of]],0)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{20D3C205-D24B-481F-A0A5-97A6101B312A}" name="DSA" displayName="DSA" ref="A2:G7" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
   <autoFilter ref="A2:G7" xr:uid="{20D3C205-D24B-481F-A0A5-97A6101B312A}"/>
   <tableColumns count="7">
@@ -3325,17 +3380,17 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F35ED7B2-2694-475F-9750-DB6006F821CB}" name="OOP_9" displayName="OOP_9" ref="A2:G5" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F35ED7B2-2694-475F-9750-DB6006F821CB}" name="OOP_9" displayName="OOP_9" ref="A2:G5" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
   <autoFilter ref="A2:G5" xr:uid="{F35ED7B2-2694-475F-9750-DB6006F821CB}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{E80B8A59-3B9F-4512-8A91-0C6601A07EE2}" name="Assessment" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{E5D6FFF2-E218-4868-ADD3-69587A76F673}" name="Type" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{59C1D46E-21B1-49C7-8032-C8F8375176BE}" name="Date" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{74073497-F8B4-4CA4-AE6C-18AF43D79BB4}" name="Weight" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{E1196646-88EC-4C14-B54C-30FABBD9067B}" name="Marks" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{F7783659-DAB3-47F3-B843-4B680178AE5A}" name="Out Of" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{63276932-3C7D-439A-979B-4B0ECD257653}" name="Percent" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{E80B8A59-3B9F-4512-8A91-0C6601A07EE2}" name="Assessment" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{E5D6FFF2-E218-4868-ADD3-69587A76F673}" name="Type" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{59C1D46E-21B1-49C7-8032-C8F8375176BE}" name="Date" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{74073497-F8B4-4CA4-AE6C-18AF43D79BB4}" name="Weight" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{E1196646-88EC-4C14-B54C-30FABBD9067B}" name="Marks" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{F7783659-DAB3-47F3-B843-4B680178AE5A}" name="Out Of" dataDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{63276932-3C7D-439A-979B-4B0ECD257653}" name="Percent" dataDxfId="57">
       <calculatedColumnFormula>IFERROR(OOP_9[[#This Row],[Marks]]/OOP_9[[#This Row],[Out Of]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3343,17 +3398,17 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B4AFA088-5628-4B0C-A947-DF271B3597BC}" name="MLFCS" displayName="MLFCS" ref="A2:G15" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B4AFA088-5628-4B0C-A947-DF271B3597BC}" name="MLFCS" displayName="MLFCS" ref="A2:G15" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
   <autoFilter ref="A2:G15" xr:uid="{B4AFA088-5628-4B0C-A947-DF271B3597BC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{15DC20F1-D841-4813-BF61-022F87C55DD2}" name="Assessment" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{98565EC1-AB66-491E-907F-60B1C3C06AED}" name="Type" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{E226E69F-80DF-46D2-B2DB-919F4093C819}" name="Date" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{14002C37-7FC0-4B1E-9971-2BD856C2B2DB}" name="Weight" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{4896E73E-0ED6-41FF-AEF7-13DD8D5F34A7}" name="Marks" dataDxfId="59"/>
-    <tableColumn id="6" xr3:uid="{1D2BE4DF-6511-493E-AE36-FF8A538CC8FF}" name="Out Of" dataDxfId="58"/>
-    <tableColumn id="7" xr3:uid="{C9A7BCBC-9AE4-4642-AEA7-952B70FD4E74}" name="Percent" dataDxfId="57">
+    <tableColumn id="1" xr3:uid="{15DC20F1-D841-4813-BF61-022F87C55DD2}" name="Assessment" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{98565EC1-AB66-491E-907F-60B1C3C06AED}" name="Type" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{E226E69F-80DF-46D2-B2DB-919F4093C819}" name="Date" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{14002C37-7FC0-4B1E-9971-2BD856C2B2DB}" name="Weight" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{4896E73E-0ED6-41FF-AEF7-13DD8D5F34A7}" name="Marks" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{1D2BE4DF-6511-493E-AE36-FF8A538CC8FF}" name="Out Of" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{C9A7BCBC-9AE4-4642-AEA7-952B70FD4E74}" name="Percent" dataDxfId="48">
       <calculatedColumnFormula>IFERROR(MLFCS[[#This Row],[Marks]]/MLFCS[[#This Row],[Out Of]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3361,17 +3416,17 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2622BBBF-6102-430C-9085-5B9BC95AF7B6}" name="OOP" displayName="OOP" ref="A2:G10" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2622BBBF-6102-430C-9085-5B9BC95AF7B6}" name="OOP" displayName="OOP" ref="A2:G10" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A2:G10" xr:uid="{2622BBBF-6102-430C-9085-5B9BC95AF7B6}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8AF69D61-70B0-4B62-8A94-84FFD4FF1E30}" name="Assessment" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{6115B625-2524-4C13-BFC6-76AD80B08F00}" name="Type" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{8E7F7644-5258-47D7-BE01-F1673A9FC9F3}" name="Date" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{A9B92261-E9DB-46C0-9F8E-65E2E3C608F6}" name="Weight" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{CB9AA16B-15AA-4947-B2F6-F7C81AF67420}" name="Marks" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{9B24B904-A5F0-44D1-ACED-E4E0338FA6DF}" name="Out Of" dataDxfId="49"/>
-    <tableColumn id="7" xr3:uid="{1A8558B6-1346-45CB-8F71-8D91CA9265F5}" name="Percent" dataDxfId="48">
+    <tableColumn id="1" xr3:uid="{8AF69D61-70B0-4B62-8A94-84FFD4FF1E30}" name="Assessment" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{6115B625-2524-4C13-BFC6-76AD80B08F00}" name="Type" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{8E7F7644-5258-47D7-BE01-F1673A9FC9F3}" name="Date" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{A9B92261-E9DB-46C0-9F8E-65E2E3C608F6}" name="Weight" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{CB9AA16B-15AA-4947-B2F6-F7C81AF67420}" name="Marks" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{9B24B904-A5F0-44D1-ACED-E4E0338FA6DF}" name="Out Of" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{1A8558B6-1346-45CB-8F71-8D91CA9265F5}" name="Percent" dataDxfId="39">
       <calculatedColumnFormula>IFERROR(OOP[[#This Row],[Marks]]/OOP[[#This Row],[Out Of]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3379,63 +3434,63 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C7F83F0-696F-4DA9-816E-95829FA77043}" name="Table1" displayName="Table1" ref="A2:E14" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C7F83F0-696F-4DA9-816E-95829FA77043}" name="Table1" displayName="Table1" ref="A2:E14" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <autoFilter ref="A2:E14" xr:uid="{8C7F83F0-696F-4DA9-816E-95829FA77043}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E14">
     <sortCondition ref="C2:C14"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8D63AB25-C4F5-4F25-B996-68DBB88FA60D}" name="Module" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{1C29305E-3227-4597-BBEC-44A2B0E4CC4F}" name="Credits" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{B27A0533-DD77-42EF-8198-23242DE0BD7D}" name="Year" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{4D8DE3E4-490E-4E79-85EE-043DF7F56F53}" name="Semester" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{7AE710B2-1596-40DF-AA87-0DC058FAF3E4}" name="Total" dataDxfId="41"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}" name="Table5" displayName="Table5" ref="A1:E27" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
-  <autoFilter ref="A1:E27" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E27">
-    <sortCondition ref="D1:D27"/>
-  </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{45B78292-D524-4642-96FC-D0DF620F1A72}" name="Assessment" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{1CA06CD8-476D-4D7E-B485-B99253CDAB02}" name="Module" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{8951D55B-B6A3-4963-B426-3FFB2CC407BA}" name="Weight" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{8DF606BA-0DF3-4A1F-93E7-16047639F3B4}" name="Release" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{7E03F087-A839-4404-AF22-222490C90F19}" name="Due" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{8D63AB25-C4F5-4F25-B996-68DBB88FA60D}" name="Module" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{1C29305E-3227-4597-BBEC-44A2B0E4CC4F}" name="Credits" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{B27A0533-DD77-42EF-8198-23242DE0BD7D}" name="Year" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{4D8DE3E4-490E-4E79-85EE-043DF7F56F53}" name="Semester" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{7AE710B2-1596-40DF-AA87-0DC058FAF3E4}" name="Total" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}" name="FYModules" displayName="FYModules" ref="A2:D16" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
-  <autoFilter ref="A2:D16" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7F7F705C-BBFB-48B0-B110-926E8E1CF419}" name="Name" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{99F42913-A4AF-439C-AFDE-38735B9668A7}" name="Semester 1" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{140A5CE5-3F0E-4A39-9385-36A06BB6BA02}" name="Semester 2" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{B24B6960-A926-4304-9414-949D710BDB68}" name="Select?" dataDxfId="28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}" name="Table5" displayName="Table5" ref="A1:E27" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="A1:E27" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E27">
+    <sortCondition ref="D1:D27"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{45B78292-D524-4642-96FC-D0DF620F1A72}" name="Assessment" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{1CA06CD8-476D-4D7E-B485-B99253CDAB02}" name="Module" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{8951D55B-B6A3-4963-B426-3FFB2CC407BA}" name="Weight" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{8DF606BA-0DF3-4A1F-93E7-16047639F3B4}" name="Release" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{7E03F087-A839-4404-AF22-222490C90F19}" name="Due" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{788C9EAD-B8A7-4E97-A5AD-984A0BD58BD0}" name="CyberSecModules" displayName="CyberSecModules" ref="A2:F11" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}" name="FYModules" displayName="FYModules" ref="A2:D16" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A2:D16" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{7F7F705C-BBFB-48B0-B110-926E8E1CF419}" name="Name" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{99F42913-A4AF-439C-AFDE-38735B9668A7}" name="Semester 1" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{140A5CE5-3F0E-4A39-9385-36A06BB6BA02}" name="Semester 2" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{B24B6960-A926-4304-9414-949D710BDB68}" name="Select?" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{788C9EAD-B8A7-4E97-A5AD-984A0BD58BD0}" name="CyberSecModules" displayName="CyberSecModules" ref="A2:F11" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A2:F11" xr:uid="{788C9EAD-B8A7-4E97-A5AD-984A0BD58BD0}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D2F9F639-DE00-4891-82FC-F2AFD9BED136}" name="Name" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{4A6B316E-C867-46CE-9E04-295046356E23}" name="Type" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{C3FB9A35-9CAA-490E-B5DD-3FB2B7EAFF24}" name="Autumn" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{7E3D05E3-EEED-4E51-9F2B-7A430A5FFFF9}" name="Spring" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{CC9BCECD-842A-4322-8A50-9292CE0AE138}" name="Summer" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{E6BCA339-BC30-44BF-9D15-3F15733224FF}" name="Select?" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{D2F9F639-DE00-4891-82FC-F2AFD9BED136}" name="Name" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{4A6B316E-C867-46CE-9E04-295046356E23}" name="Type" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{C3FB9A35-9CAA-490E-B5DD-3FB2B7EAFF24}" name="Autumn" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{7E3D05E3-EEED-4E51-9F2B-7A430A5FFFF9}" name="Spring" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{CC9BCECD-842A-4322-8A50-9292CE0AE138}" name="Summer" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{E6BCA339-BC30-44BF-9D15-3F15733224FF}" name="Select?" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3740,7 +3795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70942EC-847E-4481-B682-80D0CF4856E5}">
   <dimension ref="B3:J19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3864,7 +3919,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3969,7 +4024,10 @@
       <c r="D6" s="3">
         <v>2</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="8">
+        <f>'AI1'!K5</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -3984,7 +4042,10 @@
       <c r="D7" s="3">
         <v>2</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="8">
+        <f>FSAD!K4</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -5233,16 +5294,255 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1144FBB-AEC5-4551-9239-4C950FA59EA4}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="11" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="4">
+        <v>44610</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6">
+        <v>100</v>
+      </c>
+      <c r="G3" s="5">
+        <f>IFERROR(OOP_10[[#This Row],[Marks]]/OOP_10[[#This Row],[Out Of]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J3" s="5">
+        <f>SUMIF(OOP_10[Type],"QZ",OOP_10[Weight])</f>
+        <v>0.2</v>
+      </c>
+      <c r="K3" s="5">
+        <f>(SUMIF(OOP_10[Type],"QZ",OOP_10[Percent]))/COUNTIF(OOP_10[Type],"QZ")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="4">
+        <v>44624</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6">
+        <v>100</v>
+      </c>
+      <c r="G4" s="5">
+        <f>IFERROR(OOP_10[[#This Row],[Marks]]/OOP_10[[#This Row],[Out Of]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="5">
+        <f>SUMIF(OOP_10[Type],"EX",OOP_10[Weight])</f>
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="5">
+        <f>(SUMIF(OOP_10[Type],"EX",OOP_10[Percent]))/COUNTIF(OOP_10[Type],"EX")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="4">
+        <v>44638</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6">
+        <v>100</v>
+      </c>
+      <c r="G5" s="5">
+        <f>IFERROR(OOP_10[[#This Row],[Marks]]/OOP_10[[#This Row],[Out Of]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="5">
+        <f>SUM(J3:J4)</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="5">
+        <f>(J3*K3)+(J4*K4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="4">
+        <v>44652</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6">
+        <v>100</v>
+      </c>
+      <c r="G6" s="5">
+        <f>IFERROR(OOP_10[[#This Row],[Marks]]/OOP_10[[#This Row],[Out Of]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="4">
+        <v>44687</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6">
+        <v>100</v>
+      </c>
+      <c r="G7" s="5">
+        <f>IFERROR(OOP_10[[#This Row],[Marks]]/OOP_10[[#This Row],[Out Of]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6">
+        <v>100</v>
+      </c>
+      <c r="G8" s="5">
+        <f>IFERROR(OOP_10[[#This Row],[Marks]]/OOP_10[[#This Row],[Out Of]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -5491,8 +5791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC581F71-13EA-4CC9-8894-8953E0805102}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5511,7 +5811,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -5699,7 +5999,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E14"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6106,7 +6406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694825E1-042E-4FA4-8770-4069ED8A6469}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection sqref="A1:K10"/>
     </sheetView>
   </sheetViews>
@@ -6388,7 +6688,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update spreadsheet to include ToC
</commit_message>
<xml_diff>
--- a/resources/CS-Module-Marks-Tracker-blank.xlsx
+++ b/resources/CS-Module-Marks-Tracker-blank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\matth\Documents\school\UNI\Birmingham\Comp. Sci\CS Resources\FirstYearCSResources\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60B0E0C-8368-4161-9A75-CDCC73DFF335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5040BF69-CE77-467F-A8E4-84B208AF18E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7EF9BA6-F1C8-4970-808A-2941F4194624}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="13" xr2:uid="{B7EF9BA6-F1C8-4970-808A-2941F4194624}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="7" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="125">
   <si>
     <t>Module</t>
   </si>
@@ -416,6 +416,15 @@
   </si>
   <si>
     <t>Quizzes</t>
+  </si>
+  <si>
+    <t>W5 Assignment</t>
+  </si>
+  <si>
+    <t>W9 Assignment</t>
+  </si>
+  <si>
+    <t>W11 Assignment</t>
   </si>
 </sst>
 </file>
@@ -543,7 +552,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="93">
     <dxf>
       <fill>
         <patternFill>
@@ -620,6 +629,37 @@
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3142,23 +3182,23 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>191894</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>165875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>265386</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>124811</xdr:rowOff>
+      <xdr:colOff>657305</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>100186</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 1">
+        <xdr:cNvPr id="3" name="Rectangle 2">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C1FC84D-0528-460A-B3C4-F083645D25DA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AA0BBDB-DAD7-4ADA-A0D7-8E7C935390C3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3166,8 +3206,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="190500"/>
-          <a:ext cx="1484586" cy="505811"/>
+          <a:off x="1268219" y="1956575"/>
+          <a:ext cx="2017986" cy="505811"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3345,34 +3385,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9EA4CCE4-E406-4481-AA90-9A07CAD5BE7E}" name="OOP_10" displayName="OOP_10" ref="A2:G8" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9EA4CCE4-E406-4481-AA90-9A07CAD5BE7E}" name="AI" displayName="AI" ref="A2:G8" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91">
   <autoFilter ref="A2:G8" xr:uid="{9EA4CCE4-E406-4481-AA90-9A07CAD5BE7E}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{69A62117-FC87-4ECC-AB98-EF35B05A468E}" name="Assessment" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{60753137-725D-4636-8C02-EC3D7FD23525}" name="Type" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{05971888-5882-46B9-8195-7C40FE55BDBF}" name="Date" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{79E72D4D-8ED7-4B0C-8D4A-E1F6B54F9E04}" name="Weight" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{25BA5AEC-6E95-498F-9617-9DADAFA4F49D}" name="Marks" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{8BC298BB-3525-4A67-928C-CDEF4817E4CE}" name="Out Of" dataDxfId="76"/>
-    <tableColumn id="7" xr3:uid="{AD958F54-11F6-4131-85C7-2EB5FF82A984}" name="Percent" dataDxfId="75">
-      <calculatedColumnFormula>IFERROR(OOP_10[[#This Row],[Marks]]/OOP_10[[#This Row],[Out Of]],0)</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{69A62117-FC87-4ECC-AB98-EF35B05A468E}" name="Assessment" dataDxfId="90"/>
+    <tableColumn id="2" xr3:uid="{60753137-725D-4636-8C02-EC3D7FD23525}" name="Type" dataDxfId="89"/>
+    <tableColumn id="3" xr3:uid="{05971888-5882-46B9-8195-7C40FE55BDBF}" name="Date" dataDxfId="88"/>
+    <tableColumn id="4" xr3:uid="{79E72D4D-8ED7-4B0C-8D4A-E1F6B54F9E04}" name="Weight" dataDxfId="87"/>
+    <tableColumn id="5" xr3:uid="{25BA5AEC-6E95-498F-9617-9DADAFA4F49D}" name="Marks" dataDxfId="86"/>
+    <tableColumn id="6" xr3:uid="{8BC298BB-3525-4A67-928C-CDEF4817E4CE}" name="Out Of" dataDxfId="85"/>
+    <tableColumn id="7" xr3:uid="{AD958F54-11F6-4131-85C7-2EB5FF82A984}" name="Percent" dataDxfId="84">
+      <calculatedColumnFormula>IFERROR(AI[[#This Row],[Marks]]/AI[[#This Row],[Out Of]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{788C9EAD-B8A7-4E97-A5AD-984A0BD58BD0}" name="CyberSecModules" displayName="CyberSecModules" ref="A2:F11" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A2:F11" xr:uid="{788C9EAD-B8A7-4E97-A5AD-984A0BD58BD0}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{D2F9F639-DE00-4891-82FC-F2AFD9BED136}" name="Name" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{4A6B316E-C867-46CE-9E04-295046356E23}" name="Type" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{C3FB9A35-9CAA-490E-B5DD-3FB2B7EAFF24}" name="Autumn" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{7E3D05E3-EEED-4E51-9F2B-7A430A5FFFF9}" name="Spring" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{CC9BCECD-842A-4322-8A50-9292CE0AE138}" name="Summer" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{E6BCA339-BC30-44BF-9D15-3F15733224FF}" name="Select?" dataDxfId="20"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{20D3C205-D24B-481F-A0A5-97A6101B312A}" name="DSA" displayName="DSA" ref="A2:G7" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{20D3C205-D24B-481F-A0A5-97A6101B312A}" name="DSA" displayName="DSA" ref="A2:G7" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="A2:G7" xr:uid="{20D3C205-D24B-481F-A0A5-97A6101B312A}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2270E0A8-E28C-4AF9-BFC1-A412E0725E4C}" name="Assessment" dataDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{7052E14A-65AF-43E2-8483-D779564FD6C0}" name="Type" dataDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{63A96BCC-5661-4CA8-9927-9E1FA068D3C4}" name="Date" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{1F33FCAA-DEEE-45E2-89E6-03E71911E17F}" name="Weight" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{F1F6B912-427B-4B79-AD72-0E5794AA2EB0}" name="Marks" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{C6CD4014-F914-41A7-9044-7D2D5C20AB20}" name="Out Of" dataDxfId="67"/>
-    <tableColumn id="7" xr3:uid="{21C62A9F-30A4-4FEA-9205-6025E71D32F4}" name="Percent" dataDxfId="66">
+    <tableColumn id="1" xr3:uid="{2270E0A8-E28C-4AF9-BFC1-A412E0725E4C}" name="Assessment" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{7052E14A-65AF-43E2-8483-D779564FD6C0}" name="Type" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{63A96BCC-5661-4CA8-9927-9E1FA068D3C4}" name="Date" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{1F33FCAA-DEEE-45E2-89E6-03E71911E17F}" name="Weight" dataDxfId="78"/>
+    <tableColumn id="5" xr3:uid="{F1F6B912-427B-4B79-AD72-0E5794AA2EB0}" name="Marks" dataDxfId="77"/>
+    <tableColumn id="6" xr3:uid="{C6CD4014-F914-41A7-9044-7D2D5C20AB20}" name="Out Of" dataDxfId="76"/>
+    <tableColumn id="7" xr3:uid="{21C62A9F-30A4-4FEA-9205-6025E71D32F4}" name="Percent" dataDxfId="75">
       <calculatedColumnFormula>IFERROR(DSA[[#This Row],[Marks]]/DSA[[#This Row],[Out Of]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3381,17 +3436,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F35ED7B2-2694-475F-9750-DB6006F821CB}" name="OOP_9" displayName="OOP_9" ref="A2:G5" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F35ED7B2-2694-475F-9750-DB6006F821CB}" name="FSAD" displayName="FSAD" ref="A2:G5" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
   <autoFilter ref="A2:G5" xr:uid="{F35ED7B2-2694-475F-9750-DB6006F821CB}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{E80B8A59-3B9F-4512-8A91-0C6601A07EE2}" name="Assessment" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{E5D6FFF2-E218-4868-ADD3-69587A76F673}" name="Type" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{59C1D46E-21B1-49C7-8032-C8F8375176BE}" name="Date" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{74073497-F8B4-4CA4-AE6C-18AF43D79BB4}" name="Weight" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{E1196646-88EC-4C14-B54C-30FABBD9067B}" name="Marks" dataDxfId="59"/>
-    <tableColumn id="6" xr3:uid="{F7783659-DAB3-47F3-B843-4B680178AE5A}" name="Out Of" dataDxfId="58"/>
-    <tableColumn id="7" xr3:uid="{63276932-3C7D-439A-979B-4B0ECD257653}" name="Percent" dataDxfId="57">
-      <calculatedColumnFormula>IFERROR(OOP_9[[#This Row],[Marks]]/OOP_9[[#This Row],[Out Of]],0)</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{E80B8A59-3B9F-4512-8A91-0C6601A07EE2}" name="Assessment" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{E5D6FFF2-E218-4868-ADD3-69587A76F673}" name="Type" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{59C1D46E-21B1-49C7-8032-C8F8375176BE}" name="Date" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{74073497-F8B4-4CA4-AE6C-18AF43D79BB4}" name="Weight" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{E1196646-88EC-4C14-B54C-30FABBD9067B}" name="Marks" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{F7783659-DAB3-47F3-B843-4B680178AE5A}" name="Out Of" dataDxfId="67"/>
+    <tableColumn id="7" xr3:uid="{63276932-3C7D-439A-979B-4B0ECD257653}" name="Percent" dataDxfId="66">
+      <calculatedColumnFormula>IFERROR(FSAD[[#This Row],[Marks]]/FSAD[[#This Row],[Out Of]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3399,16 +3454,16 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B4AFA088-5628-4B0C-A947-DF271B3597BC}" name="MLFCS" displayName="MLFCS" ref="A2:G15" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B4AFA088-5628-4B0C-A947-DF271B3597BC}" name="MLFCS" displayName="MLFCS" ref="A2:G15" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
   <autoFilter ref="A2:G15" xr:uid="{B4AFA088-5628-4B0C-A947-DF271B3597BC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{15DC20F1-D841-4813-BF61-022F87C55DD2}" name="Assessment" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{98565EC1-AB66-491E-907F-60B1C3C06AED}" name="Type" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{E226E69F-80DF-46D2-B2DB-919F4093C819}" name="Date" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{14002C37-7FC0-4B1E-9971-2BD856C2B2DB}" name="Weight" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{4896E73E-0ED6-41FF-AEF7-13DD8D5F34A7}" name="Marks" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{1D2BE4DF-6511-493E-AE36-FF8A538CC8FF}" name="Out Of" dataDxfId="49"/>
-    <tableColumn id="7" xr3:uid="{C9A7BCBC-9AE4-4642-AEA7-952B70FD4E74}" name="Percent" dataDxfId="48">
+    <tableColumn id="1" xr3:uid="{15DC20F1-D841-4813-BF61-022F87C55DD2}" name="Assessment" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{98565EC1-AB66-491E-907F-60B1C3C06AED}" name="Type" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{E226E69F-80DF-46D2-B2DB-919F4093C819}" name="Date" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{14002C37-7FC0-4B1E-9971-2BD856C2B2DB}" name="Weight" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{4896E73E-0ED6-41FF-AEF7-13DD8D5F34A7}" name="Marks" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{1D2BE4DF-6511-493E-AE36-FF8A538CC8FF}" name="Out Of" dataDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{C9A7BCBC-9AE4-4642-AEA7-952B70FD4E74}" name="Percent" dataDxfId="57">
       <calculatedColumnFormula>IFERROR(MLFCS[[#This Row],[Marks]]/MLFCS[[#This Row],[Out Of]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3417,16 +3472,16 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2622BBBF-6102-430C-9085-5B9BC95AF7B6}" name="OOP" displayName="OOP" ref="A2:G10" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2622BBBF-6102-430C-9085-5B9BC95AF7B6}" name="OOP" displayName="OOP" ref="A2:G10" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
   <autoFilter ref="A2:G10" xr:uid="{2622BBBF-6102-430C-9085-5B9BC95AF7B6}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8AF69D61-70B0-4B62-8A94-84FFD4FF1E30}" name="Assessment" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{6115B625-2524-4C13-BFC6-76AD80B08F00}" name="Type" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{8E7F7644-5258-47D7-BE01-F1673A9FC9F3}" name="Date" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{A9B92261-E9DB-46C0-9F8E-65E2E3C608F6}" name="Weight" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{CB9AA16B-15AA-4947-B2F6-F7C81AF67420}" name="Marks" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{9B24B904-A5F0-44D1-ACED-E4E0338FA6DF}" name="Out Of" dataDxfId="40"/>
-    <tableColumn id="7" xr3:uid="{1A8558B6-1346-45CB-8F71-8D91CA9265F5}" name="Percent" dataDxfId="39">
+    <tableColumn id="1" xr3:uid="{8AF69D61-70B0-4B62-8A94-84FFD4FF1E30}" name="Assessment" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{6115B625-2524-4C13-BFC6-76AD80B08F00}" name="Type" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{8E7F7644-5258-47D7-BE01-F1673A9FC9F3}" name="Date" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{A9B92261-E9DB-46C0-9F8E-65E2E3C608F6}" name="Weight" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{CB9AA16B-15AA-4947-B2F6-F7C81AF67420}" name="Marks" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{9B24B904-A5F0-44D1-ACED-E4E0338FA6DF}" name="Out Of" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{1A8558B6-1346-45CB-8F71-8D91CA9265F5}" name="Percent" dataDxfId="48">
       <calculatedColumnFormula>IFERROR(OOP[[#This Row],[Marks]]/OOP[[#This Row],[Out Of]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3435,62 +3490,65 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C7F83F0-696F-4DA9-816E-95829FA77043}" name="Table1" displayName="Table1" ref="A2:E14" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
-  <autoFilter ref="A2:E14" xr:uid="{8C7F83F0-696F-4DA9-816E-95829FA77043}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E14">
-    <sortCondition ref="C2:C14"/>
-  </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8D63AB25-C4F5-4F25-B996-68DBB88FA60D}" name="Module" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{1C29305E-3227-4597-BBEC-44A2B0E4CC4F}" name="Credits" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{B27A0533-DD77-42EF-8198-23242DE0BD7D}" name="Year" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{4D8DE3E4-490E-4E79-85EE-043DF7F56F53}" name="Semester" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{7AE710B2-1596-40DF-AA87-0DC058FAF3E4}" name="Total" dataDxfId="32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{16BA8125-B1D9-4539-B13E-668F02ACD335}" name="ToC" displayName="ToC" ref="A2:G6" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A2:G6" xr:uid="{16BA8125-B1D9-4539-B13E-668F02ACD335}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{CDF6555C-D342-4021-B9FF-9231A38DA5EF}" name="Assessment" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{0A6E3F27-5B4C-4548-9B68-5286C8010E56}" name="Type" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{01393EE1-7332-41C1-8B5D-7D977756C9C5}" name="Date" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{B477AAC4-3E42-4DB0-B997-CE169F78BDCF}" name="Weight" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{2A11DED9-A358-45B0-A162-FEBB45D5F100}" name="Marks" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{719E8FEE-C849-4455-8702-29C54083DDEA}" name="Out Of" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{34631738-2C89-4800-B4BE-D5055E258300}" name="Percent" dataDxfId="11">
+      <calculatedColumnFormula>IFERROR(ToC[[#This Row],[Marks]]/ToC[[#This Row],[Out Of]],0)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}" name="Table5" displayName="Table5" ref="A1:E27" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A1:E27" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E27">
-    <sortCondition ref="D1:D27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C7F83F0-696F-4DA9-816E-95829FA77043}" name="Table1" displayName="Table1" ref="A2:E14" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+  <autoFilter ref="A2:E14" xr:uid="{8C7F83F0-696F-4DA9-816E-95829FA77043}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E14">
+    <sortCondition ref="C2:C14"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{45B78292-D524-4642-96FC-D0DF620F1A72}" name="Assessment" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{1CA06CD8-476D-4D7E-B485-B99253CDAB02}" name="Module" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{8951D55B-B6A3-4963-B426-3FFB2CC407BA}" name="Weight" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{8DF606BA-0DF3-4A1F-93E7-16047639F3B4}" name="Release" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{7E03F087-A839-4404-AF22-222490C90F19}" name="Due" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{8D63AB25-C4F5-4F25-B996-68DBB88FA60D}" name="Module" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{1C29305E-3227-4597-BBEC-44A2B0E4CC4F}" name="Credits" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{B27A0533-DD77-42EF-8198-23242DE0BD7D}" name="Year" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{4D8DE3E4-490E-4E79-85EE-043DF7F56F53}" name="Semester" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{7AE710B2-1596-40DF-AA87-0DC058FAF3E4}" name="Total" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}" name="FYModules" displayName="FYModules" ref="A2:D16" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A2:D16" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7F7F705C-BBFB-48B0-B110-926E8E1CF419}" name="Name" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{99F42913-A4AF-439C-AFDE-38735B9668A7}" name="Semester 1" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{140A5CE5-3F0E-4A39-9385-36A06BB6BA02}" name="Semester 2" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{B24B6960-A926-4304-9414-949D710BDB68}" name="Select?" dataDxfId="19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}" name="Table5" displayName="Table5" ref="A1:E27" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+  <autoFilter ref="A1:E27" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E27">
+    <sortCondition ref="D1:D27"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{45B78292-D524-4642-96FC-D0DF620F1A72}" name="Assessment" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{1CA06CD8-476D-4D7E-B485-B99253CDAB02}" name="Module" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{8951D55B-B6A3-4963-B426-3FFB2CC407BA}" name="Weight" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{8DF606BA-0DF3-4A1F-93E7-16047639F3B4}" name="Release" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{7E03F087-A839-4404-AF22-222490C90F19}" name="Due" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{788C9EAD-B8A7-4E97-A5AD-984A0BD58BD0}" name="CyberSecModules" displayName="CyberSecModules" ref="A2:F11" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A2:F11" xr:uid="{788C9EAD-B8A7-4E97-A5AD-984A0BD58BD0}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D2F9F639-DE00-4891-82FC-F2AFD9BED136}" name="Name" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{4A6B316E-C867-46CE-9E04-295046356E23}" name="Type" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{C3FB9A35-9CAA-490E-B5DD-3FB2B7EAFF24}" name="Autumn" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{7E3D05E3-EEED-4E51-9F2B-7A430A5FFFF9}" name="Spring" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{CC9BCECD-842A-4322-8A50-9292CE0AE138}" name="Summer" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{E6BCA339-BC30-44BF-9D15-3F15733224FF}" name="Select?" dataDxfId="11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}" name="FYModules" displayName="FYModules" ref="A2:D16" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="A2:D16" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{7F7F705C-BBFB-48B0-B110-926E8E1CF419}" name="Name" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{99F42913-A4AF-439C-AFDE-38735B9668A7}" name="Semester 1" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{140A5CE5-3F0E-4A39-9385-36A06BB6BA02}" name="Semester 2" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{B24B6960-A926-4304-9414-949D710BDB68}" name="Select?" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3795,7 +3853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70942EC-847E-4481-B682-80D0CF4856E5}">
   <dimension ref="B3:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3918,7 +3976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FB547B-EB02-4962-87B0-376B1EBB9A6D}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -4060,7 +4118,10 @@
       <c r="D8" s="3">
         <v>2</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="8">
+        <f>ToC!K5</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -5297,7 +5358,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5371,18 +5432,18 @@
         <v>100</v>
       </c>
       <c r="G3" s="5">
-        <f>IFERROR(OOP_10[[#This Row],[Marks]]/OOP_10[[#This Row],[Out Of]],0)</f>
+        <f>IFERROR(AI[[#This Row],[Marks]]/AI[[#This Row],[Out Of]],0)</f>
         <v>0</v>
       </c>
       <c r="I3" t="s">
         <v>121</v>
       </c>
       <c r="J3" s="5">
-        <f>SUMIF(OOP_10[Type],"QZ",OOP_10[Weight])</f>
+        <f>SUMIF(AI[Type],"QZ",AI[Weight])</f>
         <v>0.2</v>
       </c>
       <c r="K3" s="5">
-        <f>(SUMIF(OOP_10[Type],"QZ",OOP_10[Percent]))/COUNTIF(OOP_10[Type],"QZ")</f>
+        <f>(SUMIF(AI[Type],"QZ",AI[Percent]))/COUNTIF(AI[Type],"QZ")</f>
         <v>0</v>
       </c>
     </row>
@@ -5404,18 +5465,18 @@
         <v>100</v>
       </c>
       <c r="G4" s="5">
-        <f>IFERROR(OOP_10[[#This Row],[Marks]]/OOP_10[[#This Row],[Out Of]],0)</f>
+        <f>IFERROR(AI[[#This Row],[Marks]]/AI[[#This Row],[Out Of]],0)</f>
         <v>0</v>
       </c>
       <c r="I4" t="s">
         <v>42</v>
       </c>
       <c r="J4" s="5">
-        <f>SUMIF(OOP_10[Type],"EX",OOP_10[Weight])</f>
+        <f>SUMIF(AI[Type],"EX",AI[Weight])</f>
         <v>0.8</v>
       </c>
       <c r="K4" s="5">
-        <f>(SUMIF(OOP_10[Type],"EX",OOP_10[Percent]))/COUNTIF(OOP_10[Type],"EX")</f>
+        <f>(SUMIF(AI[Type],"EX",AI[Percent]))/COUNTIF(AI[Type],"EX")</f>
         <v>0</v>
       </c>
     </row>
@@ -5437,7 +5498,7 @@
         <v>100</v>
       </c>
       <c r="G5" s="5">
-        <f>IFERROR(OOP_10[[#This Row],[Marks]]/OOP_10[[#This Row],[Out Of]],0)</f>
+        <f>IFERROR(AI[[#This Row],[Marks]]/AI[[#This Row],[Out Of]],0)</f>
         <v>0</v>
       </c>
       <c r="I5" t="s">
@@ -5470,7 +5531,7 @@
         <v>100</v>
       </c>
       <c r="G6" s="5">
-        <f>IFERROR(OOP_10[[#This Row],[Marks]]/OOP_10[[#This Row],[Out Of]],0)</f>
+        <f>IFERROR(AI[[#This Row],[Marks]]/AI[[#This Row],[Out Of]],0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5492,7 +5553,7 @@
         <v>100</v>
       </c>
       <c r="G7" s="5">
-        <f>IFERROR(OOP_10[[#This Row],[Marks]]/OOP_10[[#This Row],[Out Of]],0)</f>
+        <f>IFERROR(AI[[#This Row],[Marks]]/AI[[#This Row],[Out Of]],0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5512,7 +5573,7 @@
         <v>100</v>
       </c>
       <c r="G8" s="5">
-        <f>IFERROR(OOP_10[[#This Row],[Marks]]/OOP_10[[#This Row],[Out Of]],0)</f>
+        <f>IFERROR(AI[[#This Row],[Marks]]/AI[[#This Row],[Out Of]],0)</f>
         <v>0</v>
       </c>
     </row>
@@ -5550,7 +5611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A89331-E514-4DF8-906F-BF617AA0186A}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
@@ -5792,7 +5853,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5867,18 +5928,18 @@
         <v>100</v>
       </c>
       <c r="G3" s="5">
-        <f>IFERROR(OOP_9[[#This Row],[Marks]]/OOP_9[[#This Row],[Out Of]],0)</f>
+        <f>IFERROR(FSAD[[#This Row],[Marks]]/FSAD[[#This Row],[Out Of]],0)</f>
         <v>0</v>
       </c>
       <c r="I3" t="s">
         <v>36</v>
       </c>
       <c r="J3" s="7">
-        <f>SUMIF(OOP_9[Type],"AS",OOP_9[Weight])</f>
+        <f>SUMIF(FSAD[Type],"AS",FSAD[Weight])</f>
         <v>1</v>
       </c>
       <c r="K3" s="7">
-        <f>(SUMIF(OOP_9[Type],"AS",OOP_9[Percent]))/COUNTIF(OOP_9[Type],"AS")</f>
+        <f>(SUMIF(FSAD[Type],"AS",FSAD[Percent]))/COUNTIF(FSAD[Type],"AS")</f>
         <v>0</v>
       </c>
     </row>
@@ -5900,7 +5961,7 @@
         <v>100</v>
       </c>
       <c r="G4" s="5">
-        <f>IFERROR(OOP_9[[#This Row],[Marks]]/OOP_9[[#This Row],[Out Of]],0)</f>
+        <f>IFERROR(FSAD[[#This Row],[Marks]]/FSAD[[#This Row],[Out Of]],0)</f>
         <v>0</v>
       </c>
       <c r="I4" t="s">
@@ -5933,7 +5994,7 @@
         <v>100</v>
       </c>
       <c r="G5" s="5">
-        <f>IFERROR(OOP_9[[#This Row],[Marks]]/OOP_9[[#This Row],[Out Of]],0)</f>
+        <f>IFERROR(FSAD[[#This Row],[Marks]]/FSAD[[#This Row],[Out Of]],0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6407,7 +6468,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection sqref="A1:K10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6685,16 +6746,230 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD6DD3F-7EDA-4652-9952-91B166EF6148}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="4">
+        <v>44623</v>
+      </c>
+      <c r="D3" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6">
+        <v>100</v>
+      </c>
+      <c r="G3" s="5">
+        <f>IFERROR(ToC[[#This Row],[Marks]]/ToC[[#This Row],[Out Of]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="5">
+        <f>SUMIF(ToC[Type],"AS",ToC[Weight])</f>
+        <v>0.2</v>
+      </c>
+      <c r="K3" s="5">
+        <f>(SUMIF(ToC[Type],"AS",ToC[Percent]))/COUNTIF(ToC[Type],"AS")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="4">
+        <v>44651</v>
+      </c>
+      <c r="D4" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6">
+        <v>100</v>
+      </c>
+      <c r="G4" s="5">
+        <f>IFERROR(ToC[[#This Row],[Marks]]/ToC[[#This Row],[Out Of]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="5">
+        <f>SUMIF(ToC[Type],"EX",ToC[Weight])</f>
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="5">
+        <f>(SUMIF(ToC[Type],"EX",ToC[Percent]))/COUNTIF(ToC[Type],"EX")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="4">
+        <v>44686</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6">
+        <v>100</v>
+      </c>
+      <c r="G5" s="5">
+        <f>IFERROR(ToC[[#This Row],[Marks]]/ToC[[#This Row],[Out Of]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="5">
+        <f>SUM(J3:J4)</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="5">
+        <f>(J3*K3)+(J4*K4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6">
+        <v>100</v>
+      </c>
+      <c r="G6" s="5">
+        <f>IFERROR(ToC[[#This Row],[Marks]]/ToC[[#This Row],[Out Of]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update marks tracker with averages
</commit_message>
<xml_diff>
--- a/resources/CS-Module-Marks-Tracker-blank.xlsx
+++ b/resources/CS-Module-Marks-Tracker-blank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\matth\Documents\school\UNI\Birmingham\Comp. Sci\CS Resources\FirstYearCSResources\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5040BF69-CE77-467F-A8E4-84B208AF18E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB09166-154D-4C06-912F-D7644C238CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="13" xr2:uid="{B7EF9BA6-F1C8-4970-808A-2941F4194624}"/>
   </bookViews>
@@ -31,6 +31,9 @@
     <sheet name="FYM-Select" sheetId="16" r:id="rId16"/>
     <sheet name="CyberSecMScModules" sheetId="17" r:id="rId17"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId18"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -50,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="127">
   <si>
     <t>Module</t>
   </si>
@@ -425,6 +428,12 @@
   </si>
   <si>
     <t>W11 Assignment</t>
+  </si>
+  <si>
+    <t>Averages</t>
+  </si>
+  <si>
+    <t>Year 3</t>
   </si>
 </sst>
 </file>
@@ -506,7 +515,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -547,120 +556,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="93">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -698,6 +602,34 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -726,6 +658,34 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -785,6 +745,58 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -3384,6 +3396,51 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Menu"/>
+      <sheetName val="AI1"/>
+      <sheetName val="DSA"/>
+      <sheetName val="FSAD"/>
+      <sheetName val="MLFCS"/>
+      <sheetName val="OOP"/>
+      <sheetName val="ToC"/>
+      <sheetName val="AI2"/>
+      <sheetName val="FP"/>
+      <sheetName val="SN"/>
+      <sheetName val="SEPP"/>
+      <sheetName val="SPCC"/>
+      <sheetName val="TP"/>
+      <sheetName val="Final"/>
+      <sheetName val="Assessments"/>
+      <sheetName val="FYM-Select"/>
+      <sheetName val="CyberSecMScModules"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9EA4CCE4-E406-4481-AA90-9A07CAD5BE7E}" name="AI" displayName="AI" ref="A2:G8" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91">
   <autoFilter ref="A2:G8" xr:uid="{9EA4CCE4-E406-4481-AA90-9A07CAD5BE7E}"/>
@@ -3403,15 +3460,15 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{788C9EAD-B8A7-4E97-A5AD-984A0BD58BD0}" name="CyberSecModules" displayName="CyberSecModules" ref="A2:F11" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{788C9EAD-B8A7-4E97-A5AD-984A0BD58BD0}" name="CyberSecModules" displayName="CyberSecModules" ref="A2:F11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A2:F11" xr:uid="{788C9EAD-B8A7-4E97-A5AD-984A0BD58BD0}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D2F9F639-DE00-4891-82FC-F2AFD9BED136}" name="Name" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{4A6B316E-C867-46CE-9E04-295046356E23}" name="Type" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{C3FB9A35-9CAA-490E-B5DD-3FB2B7EAFF24}" name="Autumn" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{7E3D05E3-EEED-4E51-9F2B-7A430A5FFFF9}" name="Spring" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{CC9BCECD-842A-4322-8A50-9292CE0AE138}" name="Summer" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{E6BCA339-BC30-44BF-9D15-3F15733224FF}" name="Select?" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{D2F9F639-DE00-4891-82FC-F2AFD9BED136}" name="Name" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{4A6B316E-C867-46CE-9E04-295046356E23}" name="Type" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{C3FB9A35-9CAA-490E-B5DD-3FB2B7EAFF24}" name="Autumn" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{7E3D05E3-EEED-4E51-9F2B-7A430A5FFFF9}" name="Spring" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{CC9BCECD-842A-4322-8A50-9292CE0AE138}" name="Summer" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{E6BCA339-BC30-44BF-9D15-3F15733224FF}" name="Select?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3490,16 +3547,16 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{16BA8125-B1D9-4539-B13E-668F02ACD335}" name="ToC" displayName="ToC" ref="A2:G6" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{16BA8125-B1D9-4539-B13E-668F02ACD335}" name="ToC" displayName="ToC" ref="A2:G6" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A2:G6" xr:uid="{16BA8125-B1D9-4539-B13E-668F02ACD335}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{CDF6555C-D342-4021-B9FF-9231A38DA5EF}" name="Assessment" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{0A6E3F27-5B4C-4548-9B68-5286C8010E56}" name="Type" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{01393EE1-7332-41C1-8B5D-7D977756C9C5}" name="Date" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{B477AAC4-3E42-4DB0-B997-CE169F78BDCF}" name="Weight" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{2A11DED9-A358-45B0-A162-FEBB45D5F100}" name="Marks" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{719E8FEE-C849-4455-8702-29C54083DDEA}" name="Out Of" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{34631738-2C89-4800-B4BE-D5055E258300}" name="Percent" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{CDF6555C-D342-4021-B9FF-9231A38DA5EF}" name="Assessment" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{0A6E3F27-5B4C-4548-9B68-5286C8010E56}" name="Type" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{01393EE1-7332-41C1-8B5D-7D977756C9C5}" name="Date" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{B477AAC4-3E42-4DB0-B997-CE169F78BDCF}" name="Weight" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{2A11DED9-A358-45B0-A162-FEBB45D5F100}" name="Marks" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{719E8FEE-C849-4455-8702-29C54083DDEA}" name="Out Of" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{34631738-2C89-4800-B4BE-D5055E258300}" name="Percent" dataDxfId="39">
       <calculatedColumnFormula>IFERROR(ToC[[#This Row],[Marks]]/ToC[[#This Row],[Out Of]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3508,47 +3565,47 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C7F83F0-696F-4DA9-816E-95829FA77043}" name="Table1" displayName="Table1" ref="A2:E14" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C7F83F0-696F-4DA9-816E-95829FA77043}" name="Table1" displayName="Table1" ref="A2:E14" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A2:E14" xr:uid="{8C7F83F0-696F-4DA9-816E-95829FA77043}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E14">
     <sortCondition ref="C2:C14"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8D63AB25-C4F5-4F25-B996-68DBB88FA60D}" name="Module" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{1C29305E-3227-4597-BBEC-44A2B0E4CC4F}" name="Credits" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{B27A0533-DD77-42EF-8198-23242DE0BD7D}" name="Year" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{4D8DE3E4-490E-4E79-85EE-043DF7F56F53}" name="Semester" dataDxfId="42"/>
-    <tableColumn id="5" xr3:uid="{7AE710B2-1596-40DF-AA87-0DC058FAF3E4}" name="Total" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{8D63AB25-C4F5-4F25-B996-68DBB88FA60D}" name="Module" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{1C29305E-3227-4597-BBEC-44A2B0E4CC4F}" name="Credits" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{B27A0533-DD77-42EF-8198-23242DE0BD7D}" name="Year" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{4D8DE3E4-490E-4E79-85EE-043DF7F56F53}" name="Semester" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{7AE710B2-1596-40DF-AA87-0DC058FAF3E4}" name="Total" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}" name="Table5" displayName="Table5" ref="A1:E27" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}" name="Table5" displayName="Table5" ref="A1:E27" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:E27" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E27">
     <sortCondition ref="D1:D27"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{45B78292-D524-4642-96FC-D0DF620F1A72}" name="Assessment" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{1CA06CD8-476D-4D7E-B485-B99253CDAB02}" name="Module" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{8951D55B-B6A3-4963-B426-3FFB2CC407BA}" name="Weight" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{8DF606BA-0DF3-4A1F-93E7-16047639F3B4}" name="Release" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{7E03F087-A839-4404-AF22-222490C90F19}" name="Due" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{45B78292-D524-4642-96FC-D0DF620F1A72}" name="Assessment" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{1CA06CD8-476D-4D7E-B485-B99253CDAB02}" name="Module" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{8951D55B-B6A3-4963-B426-3FFB2CC407BA}" name="Weight" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{8DF606BA-0DF3-4A1F-93E7-16047639F3B4}" name="Release" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{7E03F087-A839-4404-AF22-222490C90F19}" name="Due" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}" name="FYModules" displayName="FYModules" ref="A2:D16" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}" name="FYModules" displayName="FYModules" ref="A2:D16" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A2:D16" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7F7F705C-BBFB-48B0-B110-926E8E1CF419}" name="Name" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{99F42913-A4AF-439C-AFDE-38735B9668A7}" name="Semester 1" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{140A5CE5-3F0E-4A39-9385-36A06BB6BA02}" name="Semester 2" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{B24B6960-A926-4304-9414-949D710BDB68}" name="Select?" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{7F7F705C-BBFB-48B0-B110-926E8E1CF419}" name="Name" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{99F42913-A4AF-439C-AFDE-38735B9668A7}" name="Semester 1" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{140A5CE5-3F0E-4A39-9385-36A06BB6BA02}" name="Semester 2" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{B24B6960-A926-4304-9414-949D710BDB68}" name="Select?" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3974,7 +4031,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FB547B-EB02-4962-87B0-376B1EBB9A6D}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:E1"/>
@@ -3987,9 +4044,10 @@
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>6</v>
       </c>
@@ -3998,7 +4056,7 @@
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -4015,7 +4073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
@@ -4033,7 +4091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>10</v>
       </c>
@@ -4050,8 +4108,12 @@
         <f>MLFCS!K6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -4068,8 +4130,15 @@
         <f>OOP!K5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="7">
+        <f>SUMIF(Table1[Year],"1",Table1[Total])/COUNTIF(Table1[Year],"1")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
@@ -4086,8 +4155,15 @@
         <f>'AI1'!K5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="7">
+        <f>(SUMIFS(Table1[Total], Table1[Semester],"1",Table1[Year],"1"))/(COUNTIFS(Table1[Semester],"1",Table1[Year],"1"))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>9</v>
       </c>
@@ -4104,8 +4180,15 @@
         <f>FSAD!K4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="7">
+        <f>(SUMIFS(Table1[Total], Table1[Semester],"2",Table1[Year],"1"))/(COUNTIFS(Table1[Semester],"2",Table1[Year],"1"))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
@@ -4122,8 +4205,15 @@
         <f>ToC!K5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="7">
+        <f>SUMIF(Table1[Year],"2",Table1[Total])/COUNTIF(Table1[Year],"2")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>14</v>
       </c>
@@ -4137,8 +4227,15 @@
         <v>1</v>
       </c>
       <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="7">
+        <f>(SUMIFS(Table1[Total], Table1[Semester],"1",Table1[Year],"2"))/(COUNTIFS(Table1[Semester],"1",Table1[Year],"2"))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>16</v>
       </c>
@@ -4152,8 +4249,15 @@
         <v>1</v>
       </c>
       <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="7">
+        <f>(SUMIFS(Table1[Total],Table1[Semester],"2",Table1[Year],"2"))/(COUNTIFS(Table1[Semester],"2",Table1[Year],"2"))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>17</v>
       </c>
@@ -4167,8 +4271,15 @@
         <v>1</v>
       </c>
       <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>126</v>
+      </c>
+      <c r="H11" s="7">
+        <f>IFERROR((SUMIF(Table1[Year],"3",Table1[Total])/COUNTIF(Table1[Year],"3")),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>13</v>
       </c>
@@ -4182,8 +4293,12 @@
         <v>2</v>
       </c>
       <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -4197,8 +4312,12 @@
         <v>2</v>
       </c>
       <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>18</v>
       </c>
@@ -4214,17 +4333,18 @@
       <c r="E14" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E14">
-    <cfRule type="containsBlanks" dxfId="10" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="38" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="37" priority="3" operator="greaterThanOrEqual">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="lessThan">
       <formula>0.4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5002,18 +5122,18 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="equal">
       <formula>120</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="6" priority="4" operator="notContains" text="120">
+    <cfRule type="notContainsText" dxfId="20" priority="4" operator="notContains" text="120">
       <formula>ISERROR(SEARCH("120",G5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G4">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="notEqual">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>60</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5330,18 +5450,18 @@
     <mergeCell ref="H2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>180</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>180</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>60</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
change assignment totals for ai
</commit_message>
<xml_diff>
--- a/resources/CS-Module-Marks-Tracker-blank.xlsx
+++ b/resources/CS-Module-Marks-Tracker-blank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\matth\Documents\school\UNI\Birmingham\Comp. Sci\CS Resources\FirstYearCSResources\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB09166-154D-4C06-912F-D7644C238CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE0706D-2922-4A95-9830-C0889963E492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="13" xr2:uid="{B7EF9BA6-F1C8-4970-808A-2941F4194624}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="13" xr2:uid="{B7EF9BA6-F1C8-4970-808A-2941F4194624}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="7" r:id="rId1"/>
@@ -31,9 +31,6 @@
     <sheet name="FYM-Select" sheetId="16" r:id="rId16"/>
     <sheet name="CyberSecMScModules" sheetId="17" r:id="rId17"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId18"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -3396,51 +3393,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Menu"/>
-      <sheetName val="AI1"/>
-      <sheetName val="DSA"/>
-      <sheetName val="FSAD"/>
-      <sheetName val="MLFCS"/>
-      <sheetName val="OOP"/>
-      <sheetName val="ToC"/>
-      <sheetName val="AI2"/>
-      <sheetName val="FP"/>
-      <sheetName val="SN"/>
-      <sheetName val="SEPP"/>
-      <sheetName val="SPCC"/>
-      <sheetName val="TP"/>
-      <sheetName val="Final"/>
-      <sheetName val="Assessments"/>
-      <sheetName val="FYM-Select"/>
-      <sheetName val="CyberSecMScModules"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9EA4CCE4-E406-4481-AA90-9A07CAD5BE7E}" name="AI" displayName="AI" ref="A2:G8" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91">
   <autoFilter ref="A2:G8" xr:uid="{9EA4CCE4-E406-4481-AA90-9A07CAD5BE7E}"/>
@@ -5478,7 +5430,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5549,7 +5501,7 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="G3" s="5">
         <f>IFERROR(AI[[#This Row],[Marks]]/AI[[#This Row],[Out Of]],0)</f>
@@ -5582,7 +5534,7 @@
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="G4" s="5">
         <f>IFERROR(AI[[#This Row],[Marks]]/AI[[#This Row],[Out Of]],0)</f>
@@ -5615,7 +5567,7 @@
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="G5" s="5">
         <f>IFERROR(AI[[#This Row],[Marks]]/AI[[#This Row],[Out Of]],0)</f>
@@ -5648,7 +5600,7 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="G6" s="5">
         <f>IFERROR(AI[[#This Row],[Marks]]/AI[[#This Row],[Out Of]],0)</f>
@@ -5670,7 +5622,7 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="G7" s="5">
         <f>IFERROR(AI[[#This Row],[Marks]]/AI[[#This Row],[Out Of]],0)</f>

</xml_diff>

<commit_message>
fix ToC assignment totals
</commit_message>
<xml_diff>
--- a/resources/CS-Module-Marks-Tracker-blank.xlsx
+++ b/resources/CS-Module-Marks-Tracker-blank.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\matth\Documents\school\UNI\Birmingham\Comp. Sci\CS Resources\FirstYearCSResources\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE0706D-2922-4A95-9830-C0889963E492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EEAD2B-0226-4A72-9E2B-37498DB80EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="13" xr2:uid="{B7EF9BA6-F1C8-4970-808A-2941F4194624}"/>
   </bookViews>
@@ -6893,7 +6893,7 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G3" s="5">
         <f>IFERROR(ToC[[#This Row],[Marks]]/ToC[[#This Row],[Out Of]],0)</f>
@@ -6926,7 +6926,7 @@
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G4" s="5">
         <f>IFERROR(ToC[[#This Row],[Marks]]/ToC[[#This Row],[Out Of]],0)</f>
@@ -6959,7 +6959,7 @@
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G5" s="5">
         <f>IFERROR(ToC[[#This Row],[Marks]]/ToC[[#This Row],[Out Of]],0)</f>

</xml_diff>

<commit_message>
fix tracker exam marks
</commit_message>
<xml_diff>
--- a/resources/CS-Module-Marks-Tracker-blank.xlsx
+++ b/resources/CS-Module-Marks-Tracker-blank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\matth\Documents\school\UNI\Birmingham\Comp. Sci\CS Resources\FirstYearCSResources\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2000F798-68B5-4E3C-8225-D5CD9602C7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D651E7-C077-46C7-AD72-A8B511846442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="13" xr2:uid="{B7EF9BA6-F1C8-4970-808A-2941F4194624}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="13" xr2:uid="{B7EF9BA6-F1C8-4970-808A-2941F4194624}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="7" r:id="rId1"/>
@@ -620,9 +620,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -910,6 +907,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3640,15 +3640,15 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{788C9EAD-B8A7-4E97-A5AD-984A0BD58BD0}" name="CyberSecModules" displayName="CyberSecModules" ref="A2:F11" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{788C9EAD-B8A7-4E97-A5AD-984A0BD58BD0}" name="CyberSecModules" displayName="CyberSecModules" ref="A2:F11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A2:F11" xr:uid="{788C9EAD-B8A7-4E97-A5AD-984A0BD58BD0}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D2F9F639-DE00-4891-82FC-F2AFD9BED136}" name="Name" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{4A6B316E-C867-46CE-9E04-295046356E23}" name="Type" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{C3FB9A35-9CAA-490E-B5DD-3FB2B7EAFF24}" name="Autumn" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{7E3D05E3-EEED-4E51-9F2B-7A430A5FFFF9}" name="Spring" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{CC9BCECD-842A-4322-8A50-9292CE0AE138}" name="Summer" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{E6BCA339-BC30-44BF-9D15-3F15733224FF}" name="Select?" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{D2F9F639-DE00-4891-82FC-F2AFD9BED136}" name="Name" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{4A6B316E-C867-46CE-9E04-295046356E23}" name="Type" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{C3FB9A35-9CAA-490E-B5DD-3FB2B7EAFF24}" name="Autumn" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{7E3D05E3-EEED-4E51-9F2B-7A430A5FFFF9}" name="Spring" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{CC9BCECD-842A-4322-8A50-9292CE0AE138}" name="Summer" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{E6BCA339-BC30-44BF-9D15-3F15733224FF}" name="Select?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3677,12 +3677,12 @@
   <autoFilter ref="A2:G5" xr:uid="{F35ED7B2-2694-475F-9750-DB6006F821CB}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{E80B8A59-3B9F-4512-8A91-0C6601A07EE2}" name="Assessment" dataDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{E5D6FFF2-E218-4868-ADD3-69587A76F673}" name="Type" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{59C1D46E-21B1-49C7-8032-C8F8375176BE}" name="Date" dataDxfId="71"/>
-    <tableColumn id="4" xr3:uid="{74073497-F8B4-4CA4-AE6C-18AF43D79BB4}" name="Weight" dataDxfId="70"/>
-    <tableColumn id="5" xr3:uid="{E1196646-88EC-4C14-B54C-30FABBD9067B}" name="Marks" dataDxfId="69"/>
-    <tableColumn id="6" xr3:uid="{F7783659-DAB3-47F3-B843-4B680178AE5A}" name="Out Of" dataDxfId="68"/>
-    <tableColumn id="7" xr3:uid="{63276932-3C7D-439A-979B-4B0ECD257653}" name="Percent" dataDxfId="67">
+    <tableColumn id="2" xr3:uid="{E5D6FFF2-E218-4868-ADD3-69587A76F673}" name="Type" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{59C1D46E-21B1-49C7-8032-C8F8375176BE}" name="Date" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{74073497-F8B4-4CA4-AE6C-18AF43D79BB4}" name="Weight" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{E1196646-88EC-4C14-B54C-30FABBD9067B}" name="Marks" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{F7783659-DAB3-47F3-B843-4B680178AE5A}" name="Out Of" dataDxfId="67"/>
+    <tableColumn id="7" xr3:uid="{63276932-3C7D-439A-979B-4B0ECD257653}" name="Percent" dataDxfId="66">
       <calculatedColumnFormula>IFERROR(FSAD[[#This Row],[Marks]]/FSAD[[#This Row],[Out Of]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3691,16 +3691,16 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B4AFA088-5628-4B0C-A947-DF271B3597BC}" name="MLFCS" displayName="MLFCS" ref="A2:G15" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B4AFA088-5628-4B0C-A947-DF271B3597BC}" name="MLFCS" displayName="MLFCS" ref="A2:G15" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
   <autoFilter ref="A2:G15" xr:uid="{B4AFA088-5628-4B0C-A947-DF271B3597BC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{15DC20F1-D841-4813-BF61-022F87C55DD2}" name="Assessment" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{98565EC1-AB66-491E-907F-60B1C3C06AED}" name="Type" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{E226E69F-80DF-46D2-B2DB-919F4093C819}" name="Date" dataDxfId="62"/>
-    <tableColumn id="4" xr3:uid="{14002C37-7FC0-4B1E-9971-2BD856C2B2DB}" name="Weight" dataDxfId="61"/>
-    <tableColumn id="5" xr3:uid="{4896E73E-0ED6-41FF-AEF7-13DD8D5F34A7}" name="Marks" dataDxfId="60"/>
-    <tableColumn id="6" xr3:uid="{1D2BE4DF-6511-493E-AE36-FF8A538CC8FF}" name="Out Of" dataDxfId="59"/>
-    <tableColumn id="7" xr3:uid="{C9A7BCBC-9AE4-4642-AEA7-952B70FD4E74}" name="Percent" dataDxfId="58">
+    <tableColumn id="1" xr3:uid="{15DC20F1-D841-4813-BF61-022F87C55DD2}" name="Assessment" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{98565EC1-AB66-491E-907F-60B1C3C06AED}" name="Type" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{E226E69F-80DF-46D2-B2DB-919F4093C819}" name="Date" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{14002C37-7FC0-4B1E-9971-2BD856C2B2DB}" name="Weight" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{4896E73E-0ED6-41FF-AEF7-13DD8D5F34A7}" name="Marks" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{1D2BE4DF-6511-493E-AE36-FF8A538CC8FF}" name="Out Of" dataDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{C9A7BCBC-9AE4-4642-AEA7-952B70FD4E74}" name="Percent" dataDxfId="57">
       <calculatedColumnFormula>IFERROR(MLFCS[[#This Row],[Marks]]/MLFCS[[#This Row],[Out Of]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3709,16 +3709,16 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2622BBBF-6102-430C-9085-5B9BC95AF7B6}" name="OOP" displayName="OOP" ref="A2:G10" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2622BBBF-6102-430C-9085-5B9BC95AF7B6}" name="OOP" displayName="OOP" ref="A2:G10" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
   <autoFilter ref="A2:G10" xr:uid="{2622BBBF-6102-430C-9085-5B9BC95AF7B6}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8AF69D61-70B0-4B62-8A94-84FFD4FF1E30}" name="Assessment" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{6115B625-2524-4C13-BFC6-76AD80B08F00}" name="Type" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{8E7F7644-5258-47D7-BE01-F1673A9FC9F3}" name="Date" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{A9B92261-E9DB-46C0-9F8E-65E2E3C608F6}" name="Weight" dataDxfId="52"/>
-    <tableColumn id="5" xr3:uid="{CB9AA16B-15AA-4947-B2F6-F7C81AF67420}" name="Marks" dataDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{9B24B904-A5F0-44D1-ACED-E4E0338FA6DF}" name="Out Of" dataDxfId="50"/>
-    <tableColumn id="7" xr3:uid="{1A8558B6-1346-45CB-8F71-8D91CA9265F5}" name="Percent" dataDxfId="49">
+    <tableColumn id="1" xr3:uid="{8AF69D61-70B0-4B62-8A94-84FFD4FF1E30}" name="Assessment" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{6115B625-2524-4C13-BFC6-76AD80B08F00}" name="Type" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{8E7F7644-5258-47D7-BE01-F1673A9FC9F3}" name="Date" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{A9B92261-E9DB-46C0-9F8E-65E2E3C608F6}" name="Weight" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{CB9AA16B-15AA-4947-B2F6-F7C81AF67420}" name="Marks" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{9B24B904-A5F0-44D1-ACED-E4E0338FA6DF}" name="Out Of" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{1A8558B6-1346-45CB-8F71-8D91CA9265F5}" name="Percent" dataDxfId="48">
       <calculatedColumnFormula>IFERROR(OOP[[#This Row],[Marks]]/OOP[[#This Row],[Out Of]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3727,16 +3727,16 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{16BA8125-B1D9-4539-B13E-668F02ACD335}" name="ToC" displayName="ToC" ref="A2:G6" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{16BA8125-B1D9-4539-B13E-668F02ACD335}" name="ToC" displayName="ToC" ref="A2:G6" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A2:G6" xr:uid="{16BA8125-B1D9-4539-B13E-668F02ACD335}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{CDF6555C-D342-4021-B9FF-9231A38DA5EF}" name="Assessment" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{0A6E3F27-5B4C-4548-9B68-5286C8010E56}" name="Type" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{01393EE1-7332-41C1-8B5D-7D977756C9C5}" name="Date" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{B477AAC4-3E42-4DB0-B997-CE169F78BDCF}" name="Weight" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{2A11DED9-A358-45B0-A162-FEBB45D5F100}" name="Marks" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{719E8FEE-C849-4455-8702-29C54083DDEA}" name="Out Of" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{34631738-2C89-4800-B4BE-D5055E258300}" name="Percent" dataDxfId="40">
+    <tableColumn id="1" xr3:uid="{CDF6555C-D342-4021-B9FF-9231A38DA5EF}" name="Assessment" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{0A6E3F27-5B4C-4548-9B68-5286C8010E56}" name="Type" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{01393EE1-7332-41C1-8B5D-7D977756C9C5}" name="Date" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{B477AAC4-3E42-4DB0-B997-CE169F78BDCF}" name="Weight" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{2A11DED9-A358-45B0-A162-FEBB45D5F100}" name="Marks" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{719E8FEE-C849-4455-8702-29C54083DDEA}" name="Out Of" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{34631738-2C89-4800-B4BE-D5055E258300}" name="Percent" dataDxfId="39">
       <calculatedColumnFormula>IFERROR(ToC[[#This Row],[Marks]]/ToC[[#This Row],[Out Of]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3745,47 +3745,47 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C7F83F0-696F-4DA9-816E-95829FA77043}" name="Table1" displayName="Table1" ref="A2:E14" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C7F83F0-696F-4DA9-816E-95829FA77043}" name="Table1" displayName="Table1" ref="A2:E14" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A2:E14" xr:uid="{8C7F83F0-696F-4DA9-816E-95829FA77043}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E14">
     <sortCondition ref="C2:C14"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8D63AB25-C4F5-4F25-B996-68DBB88FA60D}" name="Module" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{1C29305E-3227-4597-BBEC-44A2B0E4CC4F}" name="Credits" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{B27A0533-DD77-42EF-8198-23242DE0BD7D}" name="Year" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{4D8DE3E4-490E-4E79-85EE-043DF7F56F53}" name="Semester" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{7AE710B2-1596-40DF-AA87-0DC058FAF3E4}" name="Total" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{8D63AB25-C4F5-4F25-B996-68DBB88FA60D}" name="Module" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{1C29305E-3227-4597-BBEC-44A2B0E4CC4F}" name="Credits" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{B27A0533-DD77-42EF-8198-23242DE0BD7D}" name="Year" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{4D8DE3E4-490E-4E79-85EE-043DF7F56F53}" name="Semester" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{7AE710B2-1596-40DF-AA87-0DC058FAF3E4}" name="Total" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}" name="Table5" displayName="Table5" ref="A1:E27" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}" name="Table5" displayName="Table5" ref="A1:E27" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:E27" xr:uid="{C2292A9A-0DCA-4512-A38F-6D0D6C40C4F6}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E27">
     <sortCondition ref="D1:D27"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{45B78292-D524-4642-96FC-D0DF620F1A72}" name="Assessment" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{1CA06CD8-476D-4D7E-B485-B99253CDAB02}" name="Module" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{8951D55B-B6A3-4963-B426-3FFB2CC407BA}" name="Weight" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{8DF606BA-0DF3-4A1F-93E7-16047639F3B4}" name="Release" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{7E03F087-A839-4404-AF22-222490C90F19}" name="Due" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{45B78292-D524-4642-96FC-D0DF620F1A72}" name="Assessment" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{1CA06CD8-476D-4D7E-B485-B99253CDAB02}" name="Module" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{8951D55B-B6A3-4963-B426-3FFB2CC407BA}" name="Weight" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{8DF606BA-0DF3-4A1F-93E7-16047639F3B4}" name="Release" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{7E03F087-A839-4404-AF22-222490C90F19}" name="Due" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}" name="FYModules" displayName="FYModules" ref="A2:D16" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}" name="FYModules" displayName="FYModules" ref="A2:D16" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A2:D16" xr:uid="{AA52D200-724E-48EC-90EF-DCF7D39C9B67}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7F7F705C-BBFB-48B0-B110-926E8E1CF419}" name="Name" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{99F42913-A4AF-439C-AFDE-38735B9668A7}" name="Semester 1" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{140A5CE5-3F0E-4A39-9385-36A06BB6BA02}" name="Semester 2" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{B24B6960-A926-4304-9414-949D710BDB68}" name="Select?" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{7F7F705C-BBFB-48B0-B110-926E8E1CF419}" name="Name" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{99F42913-A4AF-439C-AFDE-38735B9668A7}" name="Semester 1" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{140A5CE5-3F0E-4A39-9385-36A06BB6BA02}" name="Semester 2" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{B24B6960-A926-4304-9414-949D710BDB68}" name="Select?" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4518,13 +4518,13 @@
     <mergeCell ref="G4:H4"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E14">
-    <cfRule type="containsBlanks" dxfId="39" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="38" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="37" priority="3" operator="greaterThanOrEqual">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="lessThan">
       <formula>0.4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5302,18 +5302,18 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="22" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="equal">
       <formula>120</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="21" priority="4" operator="notContains" text="120">
+    <cfRule type="notContainsText" dxfId="20" priority="4" operator="notContains" text="120">
       <formula>ISERROR(SEARCH("120",G5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G4">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="notEqual">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>60</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5630,18 +5630,18 @@
     <mergeCell ref="H2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>180</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>180</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="10" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>60</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5872,7 +5872,7 @@
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="G8" s="5">
         <f>IFERROR(AI[[#This Row],[Marks]]/AI[[#This Row],[Out Of]],0)</f>
@@ -7062,7 +7062,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7233,7 +7233,7 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="G6" s="5">
         <f>IFERROR(ToC[[#This Row],[Marks]]/ToC[[#This Row],[Out Of]],0)</f>

</xml_diff>